<commit_message>
fix: typos in XLS sheet
</commit_message>
<xml_diff>
--- a/spreadsheets/RLC_fix.xlsx
+++ b/spreadsheets/RLC_fix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\smaslan\data\Z\LiB\RLC-bridge-corrections\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0000D023-12F6-40F8-9A53-CA833BB16E15}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9CE81F-C8BA-4179-9561-DF88804771A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5055" yWindow="7890" windowWidth="7335" windowHeight="1035" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Measurement" sheetId="3" r:id="rId1"/>
@@ -185,9 +185,6 @@
   </si>
   <si>
     <t>Range Z</t>
-  </si>
-  <si>
-    <t>Calibration data: measured values of reference standards.</t>
   </si>
   <si>
     <t>Fixed Rs</t>
@@ -403,16 +400,10 @@
     <t>…</t>
   </si>
   <si>
-    <t>The short can be considered "ideal", so the values may remain zero and only the uncertainty estimates may be used to include them to final uncertainty budget.</t>
-  </si>
-  <si>
     <t>2) Select frequencies at which you want to measure and have available ref-Z data. This sheet contains selection made in scope of LiBforSecUse project for EIS spectroscopy.</t>
   </si>
   <si>
     <t>1) Select resistance standards to be used for calibration. Typical procedure is to pick two resistors for each physical range of instrument. That is one for bottom of the range and one for full range. Exception is the lowest range, where the bottom of the range is expected to be zero (SHORT standard).</t>
-  </si>
-  <si>
-    <t>4) Fill in the the list of chosen nominal calibration impedances to sheet "Ref Z list".</t>
   </si>
   <si>
     <t>List of used reference impedances.</t>
@@ -437,11 +428,6 @@
 Use Rs-Xs suffix "m" for milliOhms or nothing for Ohms. The sheet will recalculate. The same applies for nominal Z.
 Add or remove lines to/from bottom of the tables, but always copy formulas in whole width of the sheet (the gray area is referenced by other sheets!)
 Order of frequencies and standards and ranges is irrelevant. Other sheets will identify positions automaticaly.</t>
-  </si>
-  <si>
-    <t>3) Fill in Rs-Xs data and ascociated extended uncertainties (k = 2) for each standard. Fill in "Nominal Z" with nominal value of standard, i.e. 0m for SHORT, 1m for roughly 1mOhm standard, etc.
-The eventual residual value of SHORT standard (nominal 0 Ohm) is given as absolute value if available or at least some uncertainty should be estimated.
-The values of all other standards are given relative to SHORT or NULL standard against which they were calibrated. This should be mentioned in the calibration certificates. If the information whether it is absolute impedance or relative to SHORT is not available, then expand uncertainty by estimate of worst case residual impedance of your SHORT standard.</t>
   </si>
   <si>
     <t>f_max</t>
@@ -471,15 +457,7 @@
     <t>1) Make list of ranges, nominal values of standards and frequencies to be calibrated following the example:</t>
   </si>
   <si>
-    <t>Select only frequencies and standard nominal impedances you have available and filled in the sheet "Ref Z". This sheet will automatically try to obtain matching rows from the sheet "Ref Z", but it will not interpolate, so the frequencies and nominal Z must match exactly. It will show warning In case of missing data.</t>
-  </si>
-  <si>
     <t>2) Take the SHORT or NULL standard that was used for calibration of your reference impedances, connect to the RLC/EIS meter and perform SHORT correction. Most modern bridges should perform the SHORTing on all ranges and frequencies automatically.</t>
-  </si>
-  <si>
-    <t>3) Measure residual impedance of the connected SHORT standard to the "sh Rs-Xs" columns and include type A uncertainty (averaging is needed for best accuracy). This step is crucial, because RLC/EIS meters perform their SHORTing with one reading per frequency and range and this process is very noisy. Even just after SHORTing the instrument often shows residual Rs-Xs in tens of µOhms or even more depending on the measurement current. 
-Therefore, for best performance, it is necessary to measure residual short Rs-Xs after SHORTing procedure to this sheet and the sheet will subtract it from the main measurement in columns Rs-Xs.
-The residual SHORT measurement is not performed for the 0 Ohm range and 0 Ohm nominal (gray area). It is performed only for the yellow areas. Note it is enough to measure the SHORT residuals only once per range and it can be copied to the other nominal impedance rows of the same range as long as the measurement is performed fast in sequence.</t>
   </si>
   <si>
     <t>Std. nominal Z</t>
@@ -491,16 +469,10 @@
 Order of frequencies and standards and ranges is irrelevant. Other sheets will identify positions automaticaly.</t>
   </si>
   <si>
-    <t>This sheet uses calibration data to fix bridge errors.</t>
-  </si>
-  <si>
     <t>4) Connect first calibrating standard and measure Rs-Xs for each frequency of interest and each physical range of instrument where the standard is being used (manual ranging). Fill in the Rs-Xs and associated uncertainties to the columns Rs, Xs, ua(Rs) and ua(Xs). The averaging of measurements is crucial to reach maximum accuracy of the calibration data.</t>
   </si>
   <si>
     <t>5) Repeat process for all used calibration standards from step 4).</t>
-  </si>
-  <si>
-    <t>1) Select measurement frequency and enable manual ranging of instrument and select range appropriate for measure impedance following manual. If the manual ranging is not possible, it will be necessary to estimate which range RLS/EIS meter is using. Fill in selected range and frequency to the yellow columns.</t>
   </si>
   <si>
     <t>2) Measure Rs-Xs of the standard preferably using averaging and write results to columns Rs, Xs and type A uncertainties to ua(Rs) and ua(Xs). You can change the suffix "m" which indicates milliOhms to nothing for Ohms.</t>
@@ -509,13 +481,41 @@
     <t>3) Connect SHORT standard and measure residual Rs-Xs at the SAME RANGE and frequency as in step 2). Fill in measured Rs-Xs and associated type A uncertainties to columns "sh Rs", "sh Xs", "sh ua(Rs)" and "sh ua(Xs)".</t>
   </si>
   <si>
-    <t>4) Read the corrected result from blue columns "Fixed …". Note the expanded uncertainties "U(…)" are being calculated from reference standards uncertainties, type A uncertainties of calibration sheet and type A uncertainties of this sheet. The uncertainty does not contain effect of RLC/EIS meter non-linearity! 
-Always check the "Status" column value. If this sheet found calibration data for the measurement spot, it will show "OK". If the measured value is outside range of calibration sheet data, it will show "Extrapolated". This happens e.g. if range is 3 mOhm, calibration standards are 1 mOhm and 3 mOhm and the measure value is outside interval of &lt;3 mOhm ; 1 mOhm&gt;. If the calibration data are not found, it will show red error message. This possibly indicates wrong selection of range or frequency that was not measured in calibration sheet.</t>
-  </si>
-  <si>
     <t>Notes:
 Use Rs-Xs suffix "m" for milliOhms or nothing for Ohms. The sheet will recalculate. The same applies for nominal Z and range.
 Add or remove lines to/from bottom of the table, but always copy formulas in whole width of the sheet.</t>
+  </si>
+  <si>
+    <t>The short can be considered "ideal", so the values of impedance may remain zero and only the uncertainty estimates may be used to include them to final uncertainty budget.</t>
+  </si>
+  <si>
+    <t>3) Fill in Rs-Xs data and associated expanded uncertainties (k = 2) for each standard. Fill in "Nominal Z" with nominal value of standard, i.e. 0m for SHORT, 1m for roughly 1mOhm standard, etc.
+The eventual residual value of SHORT standard (nominal 0 Ohm) is given as absolute value if available or at least some uncertainty should be estimated.
+The values of all other standards are given relative to SHORT or NULL standard against which they were calibrated. This should be mentioned in the calibration certificate of the standards. If the information whether it is absolute impedance or relative to SHORT is not available, then expand uncertainty by estimate of worst case residual impedance of your SHORT standard.</t>
+  </si>
+  <si>
+    <t>4) Fill in the list of chosen nominal calibration impedances to sheet "Ref Z list".</t>
+  </si>
+  <si>
+    <t>RLC bridge calibration data: measured values of reference standards.</t>
+  </si>
+  <si>
+    <t>Select only frequencies and standard nominal impedances you have available and filled in the sheet "Ref Z". This sheet will automatically try to obtain matching rows from the sheet "Ref Z", but it will not interpolate, so the frequencies and nominal Z must match exactly. It will show warning in case of missing data.</t>
+  </si>
+  <si>
+    <t>3) Measure residual impedance of the connected SHORT standard to the "sh Rs-Xs" columns and include type A uncertainty (averaging is needed for best accuracy). This step is crucial, because RLC/EIS meters perform their SHORTing with one reading per frequency and range and this process is very noisy. Even just after SHORTing the instrument often shows residual Rs-Xs in tens of µOhms or even more depending on the measurement current. 
+Therefore, for best performance, it is necessary to measure residual short Rs-Xs after SHORTing procedure to this sheet and the sheet will subtract it from the main measurement in columns Rs-Xs.
+The residual SHORT measurement is not performed for the 0 Ohm range and 0 Ohm nominal (gray area). It is performed only for the yellow areas. Note it is enough to measure the SHORT residuals only once per range and frequency and it can be copied to the other nominal impedance rows of the same range as long as the measurement is performed fast in sequence.</t>
+  </si>
+  <si>
+    <t>This sheet uses calibration data to fix bridge errors for main measurements.</t>
+  </si>
+  <si>
+    <t>1) Select measurement frequency and enable manual ranging of the instrument and select range appropriate for measured impedance following manual. If the manual ranging is not possible, it will be necessary to estimate which range RLS/EIS meter is using. Fill in selected range and frequency to the yellow columns.</t>
+  </si>
+  <si>
+    <t>4) Read the corrected result from blue columns "Fixed …". Note the expanded uncertainties "U(…)" are being calculated from reference standards uncertainties, type A uncertainties of calibration sheet and type A uncertainties of this sheet. The uncertainty does not contain effect of RLC/EIS meter non-linearity! 
+Always check the "Status" column value. If this sheet found calibration data for the measurement spot, it will show "OK". If the measured value is outside range of calibration sheet data, it will show "Extrapolated". This happens e.g. if range is 3 mOhm, calibration standards are 1 mOhm and 3 mOhm and the measure value is outside interval of &lt;1 mOhm ; 3 mOhm&gt;, e.g. 3.07 mOhm or 0.997 mOhm. The correction will still work reasonaby well if the distance from calibration spots is not too big. If the calibration data are not found at all, it will show red error message. This possibly indicates wrong selection of range or frequency that was not measured in calibration sheet.</t>
   </si>
 </sst>
 </file>
@@ -1095,8 +1095,8 @@
   </sheetPr>
   <dimension ref="A1:DM115"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W21" sqref="W21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,12 +1167,12 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B3" s="59"/>
       <c r="C3" s="59"/>
@@ -1208,7 +1208,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
@@ -1225,7 +1225,7 @@
       <c r="N5" s="59"/>
       <c r="O5" s="59"/>
     </row>
-    <row r="6" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="59"/>
       <c r="B6" s="59"/>
       <c r="C6" s="59"/>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="59" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B7" s="59"/>
       <c r="C7" s="59"/>
@@ -1261,7 +1261,7 @@
       <c r="N7" s="59"/>
       <c r="O7" s="59"/>
     </row>
-    <row r="8" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="59"/>
       <c r="B8" s="59"/>
       <c r="C8" s="59"/>
@@ -1280,7 +1280,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="59" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B9" s="59"/>
       <c r="C9" s="59"/>
@@ -1297,7 +1297,7 @@
       <c r="N9" s="59"/>
       <c r="O9" s="59"/>
     </row>
-    <row r="10" spans="1:15" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="59"/>
       <c r="B10" s="59"/>
       <c r="C10" s="59"/>
@@ -1316,7 +1316,7 @@
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="59" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B12" s="59"/>
       <c r="C12" s="59"/>
@@ -1352,28 +1352,28 @@
     </row>
     <row r="18" spans="1:117" x14ac:dyDescent="0.25">
       <c r="E18" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q18" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y18" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ18" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="AR18" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="K18" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q18" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y18" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="AE18" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ18" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="AR18" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="BB18" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="CD18" t="s">
         <v>46</v>
@@ -1382,10 +1382,10 @@
         <v>47</v>
       </c>
       <c r="CY18" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="DD18" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="DD18" s="5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:117" x14ac:dyDescent="0.25">
@@ -1414,31 +1414,31 @@
       </c>
       <c r="J19" s="31"/>
       <c r="K19" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="L19" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="M19" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="L19" s="28" t="s">
+      <c r="N19" s="28" t="s">
         <v>82</v>
-      </c>
-      <c r="M19" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="N19" s="28" t="s">
-        <v>83</v>
       </c>
       <c r="O19" s="4" t="s">
         <v>12</v>
       </c>
       <c r="Q19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="R19" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="R19" s="4" t="s">
+      <c r="S19" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="S19" s="4" t="s">
+      <c r="T19" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="T19" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="U19" s="6"/>
       <c r="V19" s="55"/>
@@ -1447,39 +1447,39 @@
       </c>
       <c r="X19" s="6"/>
       <c r="Y19" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z19" s="15"/>
       <c r="AA19" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AB19" s="6"/>
       <c r="AC19" s="6"/>
       <c r="AD19" s="6"/>
       <c r="AE19" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF19" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="AG19" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="AF19" s="34" t="s">
+      <c r="AH19" s="34" t="s">
         <v>92</v>
-      </c>
-      <c r="AG19" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="AH19" s="34" t="s">
-        <v>93</v>
       </c>
       <c r="AI19" s="6"/>
       <c r="AJ19" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK19" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL19" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="AK19" s="6" t="s">
+      <c r="AM19" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="AL19" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="AM19" s="6" t="s">
-        <v>93</v>
       </c>
       <c r="AN19" s="6"/>
       <c r="AO19" s="6"/>
@@ -1506,37 +1506,37 @@
         <v>14</v>
       </c>
       <c r="AX19" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="AY19" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ19" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="AY19" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="AZ19" s="28" t="s">
-        <v>87</v>
-      </c>
       <c r="BB19" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="BC19" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="BD19" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="BC19" s="6" t="s">
+      <c r="BE19" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="BD19" s="6" t="s">
+      <c r="BF19" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="BG19" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="BE19" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="BF19" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="BG19" s="6" t="s">
+      <c r="BH19" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="BH19" s="6" t="s">
-        <v>101</v>
-      </c>
       <c r="BI19" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BJ19" s="6" t="s">
         <v>30</v>
@@ -1617,58 +1617,58 @@
         <v>17</v>
       </c>
       <c r="CN19" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="CO19" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="CP19" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="CO19" s="38" t="s">
+      <c r="CQ19" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="CP19" s="21" t="s">
+      <c r="CR19" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="CS19" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="CQ19" s="38" t="s">
+      <c r="CT19" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="CR19" s="38" t="s">
-        <v>107</v>
-      </c>
-      <c r="CS19" s="21" t="s">
+      <c r="CU19" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="CT19" s="38" t="s">
+      <c r="CV19" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="CU19" s="21" t="s">
+      <c r="CW19" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="CY19" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="CZ19" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="CV19" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="CW19" s="38" t="s">
-        <v>107</v>
-      </c>
-      <c r="CY19" s="21" t="s">
+      <c r="DA19" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="CZ19" s="21" t="s">
+      <c r="DB19" s="21" t="s">
         <v>77</v>
-      </c>
-      <c r="DA19" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="DB19" s="21" t="s">
-        <v>78</v>
       </c>
       <c r="DD19" s="21" t="s">
         <v>14</v>
       </c>
       <c r="DE19" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="DF19" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="DG19" s="28" t="s">
         <v>88</v>
-      </c>
-      <c r="DF19" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="DG19" s="28" t="s">
-        <v>89</v>
       </c>
       <c r="DH19" s="6" t="s">
         <v>8</v>
@@ -1683,7 +1683,7 @@
         <v>17</v>
       </c>
       <c r="DM19" s="49" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:117" x14ac:dyDescent="0.25">
@@ -1815,10 +1815,10 @@
         <v>4</v>
       </c>
       <c r="AY20" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AZ20" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BB20" s="1" t="s">
         <v>1</v>
@@ -1927,10 +1927,10 @@
         <v>1</v>
       </c>
       <c r="CP20" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="CQ20" s="39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="CR20" s="39" t="s">
         <v>1</v>
@@ -1942,10 +1942,10 @@
         <v>1</v>
       </c>
       <c r="CU20" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="CV20" s="39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="CW20" s="39" t="s">
         <v>1</v>
@@ -1958,10 +1958,10 @@
         <v>-</v>
       </c>
       <c r="DA20" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="DB20" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="DD20" s="22" t="s">
         <v>4</v>
@@ -1970,10 +1970,10 @@
         <v>4</v>
       </c>
       <c r="DF20" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="DG20" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="DH20" s="22" t="s">
         <v>4</v>
@@ -38217,8 +38217,8 @@
   </sheetPr>
   <dimension ref="A1:BG188"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R64" sqref="R64"/>
+    <sheetView topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38260,12 +38260,12 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -38277,7 +38277,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="57" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E4" s="57"/>
     </row>
@@ -38302,7 +38302,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="51" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D6" s="50">
         <v>0</v>
@@ -38311,7 +38311,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="60" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G6" s="60"/>
       <c r="H6" s="60"/>
@@ -38324,7 +38324,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="51" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D7" s="50">
         <v>0</v>
@@ -38344,7 +38344,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="51" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D8" s="50">
         <v>0</v>
@@ -38364,7 +38364,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="51" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D9" s="50">
         <v>0</v>
@@ -38384,7 +38384,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="53" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D10" s="52">
         <v>1</v>
@@ -38393,7 +38393,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="62" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G10" s="62"/>
       <c r="H10" s="62"/>
@@ -38406,7 +38406,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D11" s="52">
         <v>1</v>
@@ -38426,7 +38426,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="53" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D12" s="52">
         <v>1</v>
@@ -38446,7 +38446,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="53" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D13" s="52">
         <v>1</v>
@@ -38466,7 +38466,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="51" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D14" s="50">
         <v>1</v>
@@ -38475,7 +38475,7 @@
         <v>3</v>
       </c>
       <c r="F14" s="60" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G14" s="60"/>
       <c r="H14" s="60"/>
@@ -38488,7 +38488,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="51" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D15" s="50">
         <v>1</v>
@@ -38508,7 +38508,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="51" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D16" s="50">
         <v>1</v>
@@ -38528,7 +38528,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="51" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D17" s="50">
         <v>1</v>
@@ -38548,7 +38548,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="53" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D18" s="52">
         <v>3</v>
@@ -38557,7 +38557,7 @@
         <v>3</v>
       </c>
       <c r="F18" s="62" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G18" s="62"/>
       <c r="H18" s="62"/>
@@ -38570,7 +38570,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="53" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D19" s="52">
         <v>3</v>
@@ -38590,7 +38590,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="53" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D20" s="52">
         <v>3</v>
@@ -38610,7 +38610,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="53" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D21" s="52">
         <v>3</v>
@@ -38630,7 +38630,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="51" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D22" s="50">
         <v>3</v>
@@ -38639,7 +38639,7 @@
         <v>3</v>
       </c>
       <c r="F22" s="63" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G22" s="63"/>
       <c r="H22" s="63"/>
@@ -38649,7 +38649,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="59" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B24" s="59"/>
       <c r="C24" s="59"/>
@@ -38678,7 +38678,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="61" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B27" s="61"/>
       <c r="C27" s="61"/>
@@ -38690,7 +38690,7 @@
       <c r="I27" s="61"/>
       <c r="J27" s="61"/>
     </row>
-    <row r="28" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="61"/>
       <c r="B28" s="61"/>
       <c r="C28" s="61"/>
@@ -38707,7 +38707,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="61" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B30" s="61"/>
       <c r="C30" s="61"/>
@@ -38719,7 +38719,7 @@
       <c r="I30" s="61"/>
       <c r="J30" s="61"/>
     </row>
-    <row r="31" spans="1:10" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="61"/>
       <c r="B31" s="61"/>
       <c r="C31" s="61"/>
@@ -38736,7 +38736,7 @@
     </row>
     <row r="33" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A33" s="61" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B33" s="61"/>
       <c r="C33" s="61"/>
@@ -38748,7 +38748,7 @@
       <c r="I33" s="61"/>
       <c r="J33" s="61"/>
     </row>
-    <row r="34" spans="1:59" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:59" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="61"/>
       <c r="B34" s="61"/>
       <c r="C34" s="61"/>
@@ -38774,7 +38774,7 @@
     </row>
     <row r="36" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A36" s="59" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B36" s="59"/>
       <c r="C36" s="59"/>
@@ -38803,7 +38803,7 @@
     </row>
     <row r="39" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="59" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B39" s="59"/>
       <c r="C39" s="59"/>
@@ -38840,13 +38840,13 @@
     </row>
     <row r="42" spans="1:59" x14ac:dyDescent="0.25">
       <c r="F42" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="L42" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="L42" s="5" t="s">
-        <v>115</v>
-      </c>
       <c r="S42" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="X42" s="5"/>
       <c r="AG42" s="5" t="s">
@@ -38857,10 +38857,10 @@
       </c>
       <c r="AS42" s="5"/>
       <c r="AX42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="BB42" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:59" x14ac:dyDescent="0.25">
@@ -38872,7 +38872,7 @@
         <v>0</v>
       </c>
       <c r="D43" s="57" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E43" s="57"/>
       <c r="F43" s="4" t="s">
@@ -38892,16 +38892,16 @@
       </c>
       <c r="K43" s="40"/>
       <c r="L43" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="M43" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="N43" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="M43" s="26" t="s">
+      <c r="O43" s="26" t="s">
         <v>82</v>
-      </c>
-      <c r="N43" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="O43" s="26" t="s">
-        <v>83</v>
       </c>
       <c r="P43" s="4" t="s">
         <v>12</v>
@@ -38943,16 +38943,16 @@
         <v>14</v>
       </c>
       <c r="AC43" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD43" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE43" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="AD43" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="AE43" s="28" t="s">
-        <v>85</v>
-      </c>
       <c r="AG43" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AH43" s="6" t="s">
         <v>20</v>
@@ -38970,16 +38970,16 @@
         <v>17</v>
       </c>
       <c r="AM43" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AN43" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO43" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="AP43" s="28" t="s">
         <v>84</v>
-      </c>
-      <c r="AO43" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="AP43" s="28" t="s">
-        <v>85</v>
       </c>
       <c r="AR43" s="4" t="s">
         <v>19</v>
@@ -38997,28 +38997,28 @@
         <v>24</v>
       </c>
       <c r="AX43" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="AY43" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="AY43" s="38" t="s">
+      <c r="AZ43" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="AZ43" s="38" t="s">
-        <v>111</v>
-      </c>
       <c r="BB43" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="BC43" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD43" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="BC43" s="24" t="s">
+      <c r="BE43" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="BD43" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="BE43" s="24" t="s">
-        <v>78</v>
-      </c>
       <c r="BG43" s="49" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="44" spans="1:59" x14ac:dyDescent="0.25">
@@ -39104,10 +39104,10 @@
         <v>4</v>
       </c>
       <c r="AD44" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AE44" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AG44" t="s">
         <v>1</v>
@@ -39134,10 +39134,10 @@
         <v>4</v>
       </c>
       <c r="AO44" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AP44" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AR44" s="1" t="s">
         <v>1</v>
@@ -39174,10 +39174,10 @@
         <v>1</v>
       </c>
       <c r="BD44" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BE44" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:59" x14ac:dyDescent="0.25">
@@ -67716,11 +67716,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A36:J37"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A43:B43"/>
     <mergeCell ref="T43:U43"/>
     <mergeCell ref="T44:U44"/>
     <mergeCell ref="D5:E5"/>
@@ -67737,6 +67732,11 @@
     <mergeCell ref="A24:J25"/>
     <mergeCell ref="A33:J34"/>
     <mergeCell ref="A39:J40"/>
+    <mergeCell ref="A36:J37"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A43:B43"/>
   </mergeCells>
   <conditionalFormatting sqref="Q45:Q188">
     <cfRule type="containsText" dxfId="1" priority="2" stopIfTrue="1" operator="containsText" text="OK">
@@ -67760,8 +67760,8 @@
   </sheetPr>
   <dimension ref="A1:U122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U31" sqref="U31"/>
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -67785,7 +67785,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B3" s="59"/>
       <c r="C3" s="59"/>
@@ -67820,7 +67820,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B6" s="48"/>
       <c r="C6" s="48"/>
@@ -67836,7 +67836,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="57" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C7" s="57"/>
     </row>
@@ -67851,55 +67851,55 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="64" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B9" s="58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C9" s="58"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="64"/>
       <c r="B10" s="58" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C10" s="58"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="64" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B11" s="58" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C11" s="58"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="64"/>
       <c r="B12" s="58" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C12" s="58"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="64" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B13" s="58" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C13" s="58"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="64"/>
       <c r="B14" s="58" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" s="58"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="59" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="B15" s="59"/>
       <c r="C15" s="59"/>
@@ -67910,7 +67910,7 @@
       <c r="H15" s="59"/>
       <c r="I15" s="59"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="59"/>
       <c r="B16" s="59"/>
       <c r="C16" s="59"/>
@@ -67934,7 +67934,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="59" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B18" s="59"/>
       <c r="C18" s="59"/>
@@ -67969,7 +67969,7 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="59" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="B21" s="59"/>
       <c r="C21" s="59"/>
@@ -68004,7 +68004,7 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="59" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="B24" s="59"/>
       <c r="C24" s="59"/>
@@ -68028,7 +68028,7 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="59" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B26" s="59"/>
       <c r="C26" s="59"/>
@@ -68052,7 +68052,7 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
@@ -68109,7 +68109,7 @@
         <v>19</v>
       </c>
       <c r="U31" s="49" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
@@ -74080,6 +74080,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A15:I16"/>
+    <mergeCell ref="A18:I19"/>
+    <mergeCell ref="A21:I22"/>
+    <mergeCell ref="A26:I27"/>
+    <mergeCell ref="A24:I24"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="J31:K31"/>
@@ -74096,11 +74101,6 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A15:I16"/>
-    <mergeCell ref="A18:I19"/>
-    <mergeCell ref="A21:I22"/>
-    <mergeCell ref="A26:I27"/>
-    <mergeCell ref="A24:I24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -74115,7 +74115,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -74133,27 +74133,27 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -74169,7 +74169,7 @@
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="49" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -74327,14 +74327,14 @@
       </c>
       <c r="E3" s="57"/>
       <c r="F3" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G3" s="57" t="s">
         <v>28</v>
       </c>
       <c r="H3" s="57"/>
       <c r="I3" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix: more info in XLS sheet
</commit_message>
<xml_diff>
--- a/spreadsheets/RLC_fix.xlsx
+++ b/spreadsheets/RLC_fix.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\smaslan\data\Z\LiB\RLC-bridge-corrections\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9CE81F-C8BA-4179-9561-DF88804771A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD5199E-CBE0-4692-AF9B-572BCDA99980}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Measurement" sheetId="3" r:id="rId1"/>
-    <sheet name="Cal Data" sheetId="1" r:id="rId2"/>
-    <sheet name="Ref Z" sheetId="2" r:id="rId3"/>
-    <sheet name="Ref Z list" sheetId="5" r:id="rId4"/>
-    <sheet name="Ranges" sheetId="4" r:id="rId5"/>
+    <sheet name="Info" sheetId="6" r:id="rId1"/>
+    <sheet name="Measurement" sheetId="3" r:id="rId2"/>
+    <sheet name="Cal Data" sheetId="1" r:id="rId3"/>
+    <sheet name="Ref Z" sheetId="2" r:id="rId4"/>
+    <sheet name="Ref Z list" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="163">
   <si>
     <t>f</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>Nominal Z</t>
-  </si>
-  <si>
-    <t>Range list</t>
   </si>
   <si>
     <t>Range</t>
@@ -110,12 +107,6 @@
   </si>
   <si>
     <t>Reference Z (auto search from Ref Z sheet)</t>
-  </si>
-  <si>
-    <t>Min |Z|</t>
-  </si>
-  <si>
-    <t>Max |Z|</t>
   </si>
   <si>
     <t>Z tag</t>
@@ -197,12 +188,6 @@
   </si>
   <si>
     <t>Fixed U(Xs)</t>
-  </si>
-  <si>
-    <t>Min Z</t>
-  </si>
-  <si>
-    <t>Max Z</t>
   </si>
   <si>
     <t>Measured Z</t>
@@ -517,6 +502,41 @@
     <t>4) Read the corrected result from blue columns "Fixed …". Note the expanded uncertainties "U(…)" are being calculated from reference standards uncertainties, type A uncertainties of calibration sheet and type A uncertainties of this sheet. The uncertainty does not contain effect of RLC/EIS meter non-linearity! 
 Always check the "Status" column value. If this sheet found calibration data for the measurement spot, it will show "OK". If the measured value is outside range of calibration sheet data, it will show "Extrapolated". This happens e.g. if range is 3 mOhm, calibration standards are 1 mOhm and 3 mOhm and the measure value is outside interval of &lt;1 mOhm ; 3 mOhm&gt;, e.g. 3.07 mOhm or 0.997 mOhm. The correction will still work reasonaby well if the distance from calibration spots is not too big. If the calibration data are not found at all, it will show red error message. This possibly indicates wrong selection of range or frequency that was not measured in calibration sheet.</t>
   </si>
+  <si>
+    <t>This XLS sheet was made as an example how to correct reading errors of RLC bridge at low impedances.
+The calibration concepts is to measure RLC bridge error using idealy two standards per range (top and bottom of each range) in to the sheet "Cal Data".
+The sheet "Cal Data" then takes calibration data of the used impedances from sheet "Ref Z" that has to be filled in.
+The "Cal Data" sheet then calculates gain-phase errors for each row (combination of range, frequency and nominal value of calibration standard).
+The gain-phase corrections from the "Cal Data" sheet are then loaded by sheet "Measurement" and used to correct the raw RLC meter readings.</t>
+  </si>
+  <si>
+    <t>RLC corrections for LiBforSecUse project</t>
+  </si>
+  <si>
+    <t>V1.0, 2021-05-27, Czech Metrology Institute, Stanislav Maslan</t>
+  </si>
+  <si>
+    <t>EMPIR project url:</t>
+  </si>
+  <si>
+    <t>https://www.ptb.de/empir2018/de/libforsecuse/project/overview/</t>
+  </si>
+  <si>
+    <t>Validation:</t>
+  </si>
+  <si>
+    <t>Description:</t>
+  </si>
+  <si>
+    <t>The sheet functionality was validated by Octave scripts that are part of this Git project. The Octave scripts generate proceduraly some correction data and measurement data with simulated errors of the RLC bridge and user can than verify this XLS sheet corrected the values as expected.
+Note the validation does not cover uncertainty propagation yet!</t>
+  </si>
+  <si>
+    <t>This project Git:</t>
+  </si>
+  <si>
+    <t>https://github.com/smaslan/RLC-bridge-corrections</t>
+  </si>
 </sst>
 </file>
 
@@ -527,7 +547,7 @@
     <numFmt numFmtId="165" formatCode="0.000\ 00"/>
     <numFmt numFmtId="166" formatCode="0.00000000000000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -565,6 +585,25 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -624,10 +663,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -781,8 +821,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -1089,13 +1135,127 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D821F3B-7F76-41C8-81DD-6745D1AFE3EA}">
+  <sheetPr>
+    <tabColor theme="0"/>
+  </sheetPr>
+  <dimension ref="A1:J12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="66" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C3" s="67" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="67" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="66" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="59" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+    </row>
+    <row r="8" spans="1:10" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="65"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="65"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="66" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="59"/>
+    </row>
+    <row r="12" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="59"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="59"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A7:J8"/>
+    <mergeCell ref="A11:J12"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{DCCD56C8-C89D-4D04-B57B-4B5EC208F212}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{791D3D55-2B66-4B69-8B8E-207CBAC4D825}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:DM115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
@@ -1167,12 +1327,12 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B3" s="59"/>
       <c r="C3" s="59"/>
@@ -1208,7 +1368,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
@@ -1244,7 +1404,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="59" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B7" s="59"/>
       <c r="C7" s="59"/>
@@ -1280,7 +1440,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="59" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B9" s="59"/>
       <c r="C9" s="59"/>
@@ -1316,7 +1476,7 @@
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="59" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B12" s="59"/>
       <c r="C12" s="59"/>
@@ -1352,45 +1512,45 @@
     </row>
     <row r="18" spans="1:117" x14ac:dyDescent="0.25">
       <c r="E18" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="Q18" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y18" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE18" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="Y18" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="AE18" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="AJ18" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="AR18" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="BB18" s="5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="CD18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="CI18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="CY18" s="5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="DD18" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:117" x14ac:dyDescent="0.25">
       <c r="A19" s="57" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" s="57"/>
       <c r="C19" s="4" t="s">
@@ -1398,88 +1558,88 @@
       </c>
       <c r="D19" s="40"/>
       <c r="E19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="G19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="H19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="I19" s="31" t="s">
         <v>11</v>
-      </c>
-      <c r="I19" s="31" t="s">
-        <v>12</v>
       </c>
       <c r="J19" s="31"/>
       <c r="K19" s="28" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="L19" s="28" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="M19" s="28" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="N19" s="28" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="R19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="S19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="T19" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="R19" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="S19" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="T19" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="U19" s="6"/>
       <c r="V19" s="55"/>
       <c r="W19" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="X19" s="6"/>
       <c r="Y19" s="15" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="Z19" s="15"/>
       <c r="AA19" s="15" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="AB19" s="6"/>
       <c r="AC19" s="6"/>
       <c r="AD19" s="6"/>
       <c r="AE19" s="34" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="AF19" s="34" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="AG19" s="34" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="AH19" s="34" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="AI19" s="6"/>
       <c r="AJ19" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="AK19" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="AL19" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="AM19" s="6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="AN19" s="6"/>
       <c r="AO19" s="6"/>
@@ -1488,202 +1648,202 @@
       </c>
       <c r="AQ19" s="57"/>
       <c r="AR19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AS19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AT19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AV19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AW19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AS19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT19" s="4" t="s">
+      <c r="AX19" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="AY19" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="AZ19" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="BB19" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="BC19" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD19" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="BE19" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="BF19" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="BG19" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="BH19" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="BI19" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="BJ19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="BK19" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="BL19" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="BM19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="BN19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="BO19" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="BP19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="BQ19" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="BS19" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="BT19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="BU19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="BV19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="BW19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="BX19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="BY19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="BZ19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="CA19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="CB19" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="CD19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="CE19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="CF19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="CG19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="CI19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="CJ19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="CK19" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="AU19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="AV19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AW19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AX19" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="AY19" s="21" t="s">
+      <c r="CL19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="CN19" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="AZ19" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="BB19" s="6" t="s">
+      <c r="CO19" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="BC19" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="BD19" s="6" t="s">
+      <c r="CP19" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="CQ19" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="BE19" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="BF19" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="BG19" s="6" t="s">
+      <c r="CR19" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="CS19" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="CT19" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="BH19" s="6" t="s">
+      <c r="CU19" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="CV19" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="BI19" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="BJ19" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="BK19" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="BL19" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="BM19" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="BN19" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="BO19" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="BP19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="BQ19" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="BS19" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="BT19" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="BU19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="BV19" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BW19" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="BX19" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="BY19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="BZ19" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="CA19" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="CB19" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="CD19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="CE19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="CF19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="CG19" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="CI19" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="CJ19" s="6" t="s">
+      <c r="CW19" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="CY19" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="CZ19" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="DA19" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="DB19" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="DD19" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="DE19" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="DF19" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="DG19" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="DH19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="DI19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="DJ19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="DK19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="CK19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="CL19" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="CN19" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="CO19" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="CP19" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="CQ19" s="38" t="s">
-        <v>103</v>
-      </c>
-      <c r="CR19" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="CS19" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="CT19" s="38" t="s">
-        <v>104</v>
-      </c>
-      <c r="CU19" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="CV19" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="CW19" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="CY19" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="CZ19" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="DA19" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="DB19" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="DD19" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="DE19" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="DF19" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="DG19" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="DH19" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="DI19" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="DJ19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="DK19" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="DM19" s="49" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:117" x14ac:dyDescent="0.25">
@@ -1815,10 +1975,10 @@
         <v>4</v>
       </c>
       <c r="AY20" s="22" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="AZ20" s="29" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="BB20" s="1" t="s">
         <v>1</v>
@@ -1927,10 +2087,10 @@
         <v>1</v>
       </c>
       <c r="CP20" s="22" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="CQ20" s="39" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="CR20" s="39" t="s">
         <v>1</v>
@@ -1942,10 +2102,10 @@
         <v>1</v>
       </c>
       <c r="CU20" s="22" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="CV20" s="39" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="CW20" s="39" t="s">
         <v>1</v>
@@ -1958,10 +2118,10 @@
         <v>-</v>
       </c>
       <c r="DA20" s="22" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="DB20" s="22" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="DD20" s="22" t="s">
         <v>4</v>
@@ -1970,10 +2130,10 @@
         <v>4</v>
       </c>
       <c r="DF20" s="22" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="DG20" s="29" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="DH20" s="22" t="s">
         <v>4</v>
@@ -38210,15 +38370,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:BG188"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38260,24 +38420,24 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="57"/>
       <c r="C4" s="46" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="57" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E4" s="57"/>
     </row>
@@ -38302,7 +38462,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="51" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D6" s="50">
         <v>0</v>
@@ -38311,7 +38471,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="60" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G6" s="60"/>
       <c r="H6" s="60"/>
@@ -38324,7 +38484,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="51" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D7" s="50">
         <v>0</v>
@@ -38344,7 +38504,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="51" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D8" s="50">
         <v>0</v>
@@ -38364,7 +38524,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="51" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D9" s="50">
         <v>0</v>
@@ -38384,7 +38544,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="53" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D10" s="52">
         <v>1</v>
@@ -38393,7 +38553,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="62" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G10" s="62"/>
       <c r="H10" s="62"/>
@@ -38406,7 +38566,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D11" s="52">
         <v>1</v>
@@ -38426,7 +38586,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="53" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D12" s="52">
         <v>1</v>
@@ -38446,7 +38606,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="53" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D13" s="52">
         <v>1</v>
@@ -38466,7 +38626,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="51" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D14" s="50">
         <v>1</v>
@@ -38475,7 +38635,7 @@
         <v>3</v>
       </c>
       <c r="F14" s="60" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="G14" s="60"/>
       <c r="H14" s="60"/>
@@ -38488,7 +38648,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="51" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D15" s="50">
         <v>1</v>
@@ -38508,7 +38668,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="51" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D16" s="50">
         <v>1</v>
@@ -38528,7 +38688,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="51" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D17" s="50">
         <v>1</v>
@@ -38548,7 +38708,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="53" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D18" s="52">
         <v>3</v>
@@ -38557,7 +38717,7 @@
         <v>3</v>
       </c>
       <c r="F18" s="62" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="G18" s="62"/>
       <c r="H18" s="62"/>
@@ -38570,7 +38730,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="53" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D19" s="52">
         <v>3</v>
@@ -38590,7 +38750,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="53" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D20" s="52">
         <v>3</v>
@@ -38610,7 +38770,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="53" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D21" s="52">
         <v>3</v>
@@ -38630,7 +38790,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="51" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D22" s="50">
         <v>3</v>
@@ -38639,7 +38799,7 @@
         <v>3</v>
       </c>
       <c r="F22" s="63" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G22" s="63"/>
       <c r="H22" s="63"/>
@@ -38649,7 +38809,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="59" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B24" s="59"/>
       <c r="C24" s="59"/>
@@ -38678,7 +38838,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="61" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B27" s="61"/>
       <c r="C27" s="61"/>
@@ -38707,7 +38867,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="61" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B30" s="61"/>
       <c r="C30" s="61"/>
@@ -38736,7 +38896,7 @@
     </row>
     <row r="33" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A33" s="61" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B33" s="61"/>
       <c r="C33" s="61"/>
@@ -38774,7 +38934,7 @@
     </row>
     <row r="36" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A36" s="59" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B36" s="59"/>
       <c r="C36" s="59"/>
@@ -38803,7 +38963,7 @@
     </row>
     <row r="39" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="59" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B39" s="59"/>
       <c r="C39" s="59"/>
@@ -38840,88 +39000,88 @@
     </row>
     <row r="42" spans="1:59" x14ac:dyDescent="0.25">
       <c r="F42" s="5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="L42" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="S42" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="X42" s="5"/>
       <c r="AG42" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AR42" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AS42" s="5"/>
       <c r="AX42" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="BB42" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A43" s="57" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B43" s="57"/>
       <c r="C43" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D43" s="57" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E43" s="57"/>
       <c r="F43" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G43" s="4" t="s">
+      <c r="H43" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H43" s="4" t="s">
+      <c r="I43" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I43" s="4" t="s">
+      <c r="J43" s="38" t="s">
         <v>11</v>
-      </c>
-      <c r="J43" s="38" t="s">
-        <v>12</v>
       </c>
       <c r="K43" s="40"/>
       <c r="L43" s="26" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="M43" s="26" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="N43" s="26" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="O43" s="26" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="P43" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q43" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="R43" s="38"/>
       <c r="S43" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="T43" s="57" t="s">
         <v>0</v>
       </c>
       <c r="U43" s="57"/>
       <c r="V43" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="W43" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="X43" s="4" t="str">
         <f t="shared" ref="X43:AA44" si="0">F43</f>
@@ -38940,85 +39100,85 @@
         <v>ua(Xs)</v>
       </c>
       <c r="AB43" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AC43" s="28" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="AD43" s="21" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="AE43" s="28" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="AG43" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="AH43" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI43" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ43" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK43" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL43" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AM43" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN43" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO43" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP43" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR43" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AS43" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AI43" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJ43" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="AK43" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="AL43" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AM43" s="21" t="s">
+      <c r="AT43" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AU43" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AX43" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="AY43" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="AZ43" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="BB43" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="BC43" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="BD43" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="AN43" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="AO43" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="AP43" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="AR43" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AS43" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="AT43" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="AU43" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="AV43" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="AX43" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="AY43" s="38" t="s">
-        <v>109</v>
-      </c>
-      <c r="AZ43" s="38" t="s">
-        <v>110</v>
-      </c>
-      <c r="BB43" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="BC43" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="BD43" s="21" t="s">
-        <v>71</v>
-      </c>
       <c r="BE43" s="24" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="BG43" s="49" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:59" x14ac:dyDescent="0.25">
@@ -39104,10 +39264,10 @@
         <v>4</v>
       </c>
       <c r="AD44" s="22" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="AE44" s="29" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="AG44" t="s">
         <v>1</v>
@@ -39134,10 +39294,10 @@
         <v>4</v>
       </c>
       <c r="AO44" s="22" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="AP44" s="29" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="AR44" s="1" t="s">
         <v>1</v>
@@ -39174,10 +39334,10 @@
         <v>1</v>
       </c>
       <c r="BD44" s="22" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="BE44" s="25" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:59" x14ac:dyDescent="0.25">
@@ -39196,7 +39356,9 @@
       <c r="E45" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F45" s="7"/>
+      <c r="F45" s="7">
+        <v>0</v>
+      </c>
       <c r="G45" s="7">
         <v>1.9663883689823069E-3</v>
       </c>
@@ -39383,7 +39545,9 @@
         <f>E45</f>
         <v>m</v>
       </c>
-      <c r="F46" s="7"/>
+      <c r="F46" s="7">
+        <v>0</v>
+      </c>
       <c r="G46" s="7">
         <v>1.3220065619165356E-3</v>
       </c>
@@ -39570,7 +39734,9 @@
         <f t="shared" ref="E47:E62" si="36">E46</f>
         <v>m</v>
       </c>
-      <c r="F47" s="7"/>
+      <c r="F47" s="7">
+        <v>0</v>
+      </c>
       <c r="G47" s="7">
         <v>3.6972133624838628E-4</v>
       </c>
@@ -39757,7 +39923,9 @@
         <f t="shared" si="36"/>
         <v>m</v>
       </c>
-      <c r="F48" s="7"/>
+      <c r="F48" s="7">
+        <v>0</v>
+      </c>
       <c r="G48" s="7">
         <v>1.2411872657195841E-4</v>
       </c>
@@ -39944,7 +40112,9 @@
         <f t="shared" si="36"/>
         <v>m</v>
       </c>
-      <c r="F49" s="7"/>
+      <c r="F49" s="7">
+        <v>0</v>
+      </c>
       <c r="G49" s="7">
         <v>1.9609825865359925E-3</v>
       </c>
@@ -40131,7 +40301,9 @@
         <f t="shared" si="36"/>
         <v>m</v>
       </c>
-      <c r="F50" s="7"/>
+      <c r="F50" s="7">
+        <v>0</v>
+      </c>
       <c r="G50" s="7">
         <v>1.7178438584346666E-3</v>
       </c>
@@ -40318,7 +40490,9 @@
         <f t="shared" si="36"/>
         <v>m</v>
       </c>
-      <c r="F51" s="7"/>
+      <c r="F51" s="7">
+        <v>0</v>
+      </c>
       <c r="G51" s="7">
         <v>1.4433094297871074E-3</v>
       </c>
@@ -40505,7 +40679,9 @@
         <f t="shared" si="36"/>
         <v>m</v>
       </c>
-      <c r="F52" s="7"/>
+      <c r="F52" s="7">
+        <v>0</v>
+      </c>
       <c r="G52" s="7">
         <v>5.0727110872924263E-4</v>
       </c>
@@ -40692,7 +40868,9 @@
         <f t="shared" si="36"/>
         <v>m</v>
       </c>
-      <c r="F53" s="7"/>
+      <c r="F53" s="7">
+        <v>0</v>
+      </c>
       <c r="G53" s="7">
         <v>6.2869678064896527E-4</v>
       </c>
@@ -40879,7 +41057,9 @@
         <f t="shared" si="36"/>
         <v>m</v>
       </c>
-      <c r="F54" s="7"/>
+      <c r="F54" s="7">
+        <v>0</v>
+      </c>
       <c r="G54" s="7">
         <v>1.4838071625799219E-3</v>
       </c>
@@ -41066,7 +41246,9 @@
         <f t="shared" si="36"/>
         <v>m</v>
       </c>
-      <c r="F55" s="7"/>
+      <c r="F55" s="7">
+        <v>0</v>
+      </c>
       <c r="G55" s="7">
         <v>1.6960681758216071E-3</v>
       </c>
@@ -41253,7 +41435,9 @@
         <f t="shared" si="36"/>
         <v>m</v>
       </c>
-      <c r="F56" s="7"/>
+      <c r="F56" s="7">
+        <v>0</v>
+      </c>
       <c r="G56" s="7">
         <v>1.4121346399303403E-3</v>
       </c>
@@ -41440,7 +41624,9 @@
         <f t="shared" si="36"/>
         <v>m</v>
       </c>
-      <c r="F57" s="7"/>
+      <c r="F57" s="7">
+        <v>0</v>
+      </c>
       <c r="G57" s="7">
         <v>1.558244129697953E-3</v>
       </c>
@@ -41627,7 +41813,9 @@
         <f t="shared" si="36"/>
         <v>m</v>
       </c>
-      <c r="F58" s="7"/>
+      <c r="F58" s="7">
+        <v>0</v>
+      </c>
       <c r="G58" s="7">
         <v>1.6266301916568836E-5</v>
       </c>
@@ -41814,7 +42002,9 @@
         <f t="shared" si="36"/>
         <v>m</v>
       </c>
-      <c r="F59" s="7"/>
+      <c r="F59" s="7">
+        <v>0</v>
+      </c>
       <c r="G59" s="7">
         <v>8.0070539361773321E-4</v>
       </c>
@@ -42001,7 +42191,9 @@
         <f t="shared" si="36"/>
         <v>m</v>
       </c>
-      <c r="F60" s="7"/>
+      <c r="F60" s="7">
+        <v>0</v>
+      </c>
       <c r="G60" s="7">
         <v>1.5890147860507888E-3</v>
       </c>
@@ -42188,7 +42380,9 @@
         <f t="shared" si="36"/>
         <v>m</v>
       </c>
-      <c r="F61" s="7"/>
+      <c r="F61" s="7">
+        <v>0</v>
+      </c>
       <c r="G61" s="7">
         <v>7.9749250133453716E-4</v>
       </c>
@@ -67753,7 +67947,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
@@ -67780,12 +67974,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B3" s="59"/>
       <c r="C3" s="59"/>
@@ -67820,7 +68014,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B6" s="48"/>
       <c r="C6" s="48"/>
@@ -67833,10 +68027,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="57" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C7" s="57"/>
     </row>
@@ -67851,55 +68045,55 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="64" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B9" s="58" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C9" s="58"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="64"/>
       <c r="B10" s="58" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C10" s="58"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="64" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B11" s="58" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C11" s="58"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="64"/>
       <c r="B12" s="58" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C12" s="58"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="64" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B13" s="58" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C13" s="58"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="64"/>
       <c r="B14" s="58" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C14" s="58"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="59" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B15" s="59"/>
       <c r="C15" s="59"/>
@@ -67934,7 +68128,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="59" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B18" s="59"/>
       <c r="C18" s="59"/>
@@ -67969,7 +68163,7 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="59" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B21" s="59"/>
       <c r="C21" s="59"/>
@@ -68004,7 +68198,7 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="59" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B24" s="59"/>
       <c r="C24" s="59"/>
@@ -68028,7 +68222,7 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="59" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B26" s="59"/>
       <c r="C26" s="59"/>
@@ -68052,7 +68246,7 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
@@ -68064,19 +68258,19 @@
       </c>
       <c r="C31" s="57"/>
       <c r="D31" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F31" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="H31" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I31" s="40"/>
       <c r="J31" s="57" t="s">
@@ -68084,10 +68278,10 @@
       </c>
       <c r="K31" s="57"/>
       <c r="L31" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N31" s="4" t="str">
         <f t="shared" ref="N31:Q32" si="0">D31</f>
@@ -68106,10 +68300,10 @@
         <v>U(Xs)</v>
       </c>
       <c r="S31" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U31" s="49" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
@@ -74107,7 +74301,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
@@ -74133,43 +74327,43 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="57"/>
       <c r="C8" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="49" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -74289,214 +74483,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="4.5703125" customWidth="1"/>
-    <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="5" width="5.85546875" customWidth="1"/>
-    <col min="7" max="8" width="5.140625" customWidth="1"/>
-    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="57" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="57"/>
-      <c r="F3" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" s="57" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="57"/>
-      <c r="I3" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="58" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="58" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="58" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="58"/>
-      <c r="I4" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
-        <v>1</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="12">
-        <f>IF(MID(B5,1,1)="m",0.001,IF(OR(MID(B5,1,1)="u",MID(B5,1,1)="µ"),0.000001,1))*A5</f>
-        <v>1E-3</v>
-      </c>
-      <c r="D5" s="7">
-        <v>0</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="12">
-        <f>IF(MID(E5,1,1)="m",0.001,IF(OR(MID(E5,1,1)="u",MID(E5,1,1)="µ"),0.000001,1))*D5</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="7">
-        <v>1</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="12">
-        <f>IF(MID(H5,1,1)="m",0.001,IF(OR(MID(H5,1,1)="u",MID(H5,1,1)="µ"),0.000001,1))*G5</f>
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
-        <v>3</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="12">
-        <f>IF(MID(B6,1,1)="m",0.001,IF(OR(MID(B6,1,1)="u",MID(B6,1,1)="µ"),0.000001,1))*A6</f>
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="D6" s="7">
-        <v>1</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="12">
-        <f>IF(MID(E6,1,1)="m",0.001,IF(OR(MID(E6,1,1)="u",MID(E6,1,1)="µ"),0.000001,1))*D6</f>
-        <v>1E-3</v>
-      </c>
-      <c r="G6" s="7">
-        <v>3</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I6" s="12">
-        <f>IF(MID(H6,1,1)="m",0.001,IF(OR(MID(H6,1,1)="u",MID(H6,1,1)="µ"),0.000001,1))*G6</f>
-        <v>3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
-        <v>10</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="12">
-        <f>IF(MID(B7,1,1)="m",0.001,IF(OR(MID(B7,1,1)="u",MID(B7,1,1)="µ"),0.000001,1))*A7</f>
-        <v>0.01</v>
-      </c>
-      <c r="D7" s="7">
-        <v>3</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="12">
-        <f>IF(MID(E7,1,1)="m",0.001,IF(OR(MID(E7,1,1)="u",MID(E7,1,1)="µ"),0.000001,1))*D7</f>
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="G7" s="7">
-        <v>10</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I7" s="12">
-        <f>IF(MID(H7,1,1)="m",0.001,IF(OR(MID(H7,1,1)="u",MID(H7,1,1)="µ"),0.000001,1))*G7</f>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
-        <v>100</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="12">
-        <f>IF(MID(B8,1,1)="m",0.001,IF(OR(MID(B8,1,1)="u",MID(B8,1,1)="µ"),0.000001,1))*A8</f>
-        <v>0.1</v>
-      </c>
-      <c r="D8" s="7">
-        <v>10</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="12">
-        <f>IF(MID(E8,1,1)="m",0.001,IF(OR(MID(E8,1,1)="u",MID(E8,1,1)="µ"),0.000001,1))*D8</f>
-        <v>0.01</v>
-      </c>
-      <c r="G8" s="7">
-        <v>100</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I8" s="12">
-        <f>IF(MID(H8,1,1)="m",0.001,IF(OR(MID(H8,1,1)="u",MID(H8,1,1)="µ"),0.000001,1))*G8</f>
-        <v>0.1</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>